<commit_message>
QR oluşturma özelliği ekledim. Ayrıca artık revizede tcyi yanlış girince artık güzel bir şekilde bulunamadı diyor
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>tckn</t>
   </si>
@@ -24,34 +24,37 @@
     <t>Rol</t>
   </si>
   <si>
-    <t xml:space="preserve">MEHMET ALİ TULUKCU</t>
+    <t xml:space="preserve">FULYA İNCİ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takım üyesi,Yazılımcı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÖMER FARUK BORAN</t>
+  </si>
+  <si>
+    <t>Yazılımcı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MELİKE ERTAN</t>
+  </si>
+  <si>
+    <t>Yardımcı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUHAMMED ALİ KÖSEN</t>
+  </si>
+  <si>
+    <t>Araştırmacı,Yardımcı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUHAMMED GÖNEN</t>
   </si>
   <si>
     <t xml:space="preserve">Yazılımcı,Takım üyesi</t>
   </si>
   <si>
-    <t xml:space="preserve">MUSTAFA ÖZPINAR</t>
-  </si>
-  <si>
-    <t>Yardımcı,Araştırmacı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERAY EROĞLU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boş işler müdürü</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AHMET MELİH KARAUĞUZ</t>
-  </si>
-  <si>
-    <t>Yazılımcı,Yardımcı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALİ OSMAN GÜNAY</t>
-  </si>
-  <si>
-    <t>Yardımcı,Yazılımcı,Araştırmacı</t>
+    <t xml:space="preserve">FATMANUR ÖZDEMİR</t>
   </si>
 </sst>
 </file>
@@ -623,10 +626,10 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1">
-        <v>12345678900</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2">
+        <v>12345678929</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -634,10 +637,10 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1">
-        <v>12345678901</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3">
+        <v>12345678930</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -645,21 +648,21 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1">
-        <v>12345678902</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4">
+        <v>12345678931</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1">
-        <v>12345678903</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5">
+        <v>12345678932</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -667,10 +670,10 @@
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1">
-        <v>12345678904</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6">
+        <v>12345678933</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -678,9 +681,15 @@
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7">
+        <v>12345678934</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
"Nasıl çalışır?" butonu eklendi ve çoklu kayıttaki birinin zaten kayıtlı olması durumunda verdiği hatayı düzelttim artık bunları es geçiyor.
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>tckn</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t xml:space="preserve">FATMANUR ÖZDEMİR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rastgele birisi</t>
+  </si>
+  <si>
+    <t>Yazılımcı,Yardımcı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birisi daha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takım üyesi</t>
   </si>
 </sst>
 </file>
@@ -89,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -632,7 +647,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -643,7 +658,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -665,7 +680,7 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -676,7 +691,7 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -692,14 +707,26 @@
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="2">
+        <v>2313213123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1">
+        <v>6546365</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
çoklu revize dışında hepsi bitti
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -27,31 +27,31 @@
     <t xml:space="preserve">FULYA İNCİ</t>
   </si>
   <si>
-    <t xml:space="preserve">Takım üyesi,Yazılımcı</t>
+    <t xml:space="preserve">Bireysel,Takım üyesi,Yazılımcı</t>
   </si>
   <si>
     <t xml:space="preserve">ÖMER FARUK BORAN</t>
   </si>
   <si>
-    <t>Yazılımcı</t>
+    <t>Bireysel,Yazılımcı</t>
   </si>
   <si>
     <t xml:space="preserve">MELİKE ERTAN</t>
   </si>
   <si>
-    <t>Yardımcı</t>
+    <t>Bireysel,Yardımcı</t>
   </si>
   <si>
     <t xml:space="preserve">MUHAMMED ALİ KÖSEN</t>
   </si>
   <si>
-    <t>Araştırmacı,Yardımcı</t>
+    <t>Bireysel,Araştırmacı,Yardımcı</t>
   </si>
   <si>
     <t xml:space="preserve">MUHAMMED GÖNEN</t>
   </si>
   <si>
-    <t xml:space="preserve">Yazılımcı,Takım üyesi</t>
+    <t xml:space="preserve">Bireysel,Yazılımcı,Takım üyesi</t>
   </si>
   <si>
     <t xml:space="preserve">FATMANUR ÖZDEMİR</t>
@@ -60,13 +60,13 @@
     <t xml:space="preserve">Rastgele birisi</t>
   </si>
   <si>
-    <t>Yazılımcı,Yardımcı</t>
+    <t>Bireysel,Yazılımcı,Yardımcı</t>
   </si>
   <si>
     <t xml:space="preserve">Birisi daha</t>
   </si>
   <si>
-    <t xml:space="preserve">Takım üyesi</t>
+    <t xml:space="preserve">Bireysel,Takım üyesi,Araştırmacı</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
       <c r="A9" s="1">
         <v>6546365</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">

</xml_diff>